<commit_message>
Update "exp_temp_resp" to latest recommandations
</commit_message>
<xml_diff>
--- a/inst/xlsx/macrounchainedFocusGW-with-met.xlsx
+++ b/inst/xlsx/macrounchainedFocusGW-with-met.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" state="visible" r:id="rId2"/>
@@ -415,8 +415,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -741,7 +741,7 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -839,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>0.079</v>
+        <v>0.0948</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>0.49</v>
@@ -883,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>0.079</v>
+        <v>0.0948</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0.49</v>
@@ -933,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>0.079</v>
+        <v>0.0948</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>0.49</v>

</xml_diff>